<commit_message>
Update .env-example to include environment variable instructions
</commit_message>
<xml_diff>
--- a/AUTOMACAO/arquivos/P1.xlsx
+++ b/AUTOMACAO/arquivos/P1.xlsx
@@ -1,33 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28409"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win10\OneDrive\Área de Trabalho\BielziN\AUTOMACAO\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B67FB7F5-372B-4C64-B381-AF5122891EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>NOME</t>
   </si>
@@ -38,31 +50,20 @@
     <t>MENSAGEM</t>
   </si>
   <si>
-    <t>LINK DO WHATSAPP</t>
-  </si>
-  <si>
     <t>Gabriel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000000000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,19 +94,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,93 +380,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2">
-        <v>5585986877704</v>
+      <c r="B2" s="1">
+        <v>5585985010594</v>
       </c>
       <c r="C2" t="str">
         <f>"Ola, "&amp;A2&amp;" tudo bem?"</f>
         <v>Ola, Gabriel tudo bem?</v>
       </c>
-      <c r="D2" s="1" t="str">
-        <f>HYPERLINK(CONCATENATE("https://wa.me/",B2,"?text=",_xlfn.ENCODEURL(C2)))</f>
-        <v>https://wa.me/5585986877704?text=Ola%2C%20Gabriel%20tudo%20bem%3F</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2">
-        <v>5585986877704</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5585985010594</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C10" si="0">"Ola, "&amp;A3&amp;" tudo bem?"</f>
         <v>Ola, Gabriel tudo bem?</v>
       </c>
-      <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D10" si="1">HYPERLINK(CONCATENATE("https://wa.me/",B3,"?text=",_xlfn.ENCODEURL(C3)))</f>
-        <v>https://wa.me/5585986877704?text=Ola%2C%20Gabriel%20tudo%20bem%3F</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="4"/>
+    <row r="8" spans="1:3">
+      <c r="C8" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:C1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>